<commit_message>
Fixed upload & examset
</commit_message>
<xml_diff>
--- a/src/main/webapp/QuestionSample.xlsx
+++ b/src/main/webapp/QuestionSample.xlsx
@@ -120,7 +120,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RAVESH:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+To distinguish same type of questions in one subject category</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -144,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -165,30 +189,6 @@
           </rPr>
           <t xml:space="preserve">
 PassageId to be used to link questions for this passage</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>RAVESH:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-is this a graph based question?</t>
         </r>
       </text>
     </comment>
@@ -212,11 +212,35 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-How many questions are based on this paragraph</t>
+is this a graph based question?</t>
         </r>
       </text>
     </comment>
     <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RAVESH:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+How many questions are based on this paragraph</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -245,7 +269,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="48">
   <si>
     <t>Subject</t>
   </si>
@@ -380,6 +404,15 @@
   </si>
   <si>
     <t>Sample Question 1</t>
+  </si>
+  <si>
+    <t>Question SubType</t>
+  </si>
+  <si>
+    <t>TYPE_001</t>
+  </si>
+  <si>
+    <t>TYPE_002</t>
   </si>
 </sst>
 </file>
@@ -753,37 +786,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="10" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -797,73 +830,76 @@
         <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:27">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -877,67 +913,70 @@
         <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>1</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2">
+      <c r="N2" s="2"/>
+      <c r="O2" s="2">
         <v>5</v>
       </c>
-      <c r="O2" s="2">
+      <c r="P2" s="2">
         <v>60</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:27">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -951,37 +990,39 @@
         <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>5</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2">
+      <c r="N3" s="2"/>
+      <c r="O3" s="2">
         <v>5</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <v>60</v>
       </c>
-      <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -992,8 +1033,9 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
-    </row>
-    <row r="4" spans="1:26">
+      <c r="AA3" s="2"/>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1020,8 +1062,9 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
-    </row>
-    <row r="5" spans="1:26">
+      <c r="AA4" s="2"/>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1048,8 +1091,9 @@
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
-    </row>
-    <row r="6" spans="1:26">
+      <c r="AA5" s="2"/>
+    </row>
+    <row r="6" spans="1:27">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1076,8 +1120,9 @@
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
-    </row>
-    <row r="7" spans="1:26">
+      <c r="AA6" s="2"/>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1104,8 +1149,9 @@
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
-    </row>
-    <row r="8" spans="1:26">
+      <c r="AA7" s="2"/>
+    </row>
+    <row r="8" spans="1:27">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1132,8 +1178,9 @@
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
-    </row>
-    <row r="9" spans="1:26">
+      <c r="AA8" s="2"/>
+    </row>
+    <row r="9" spans="1:27">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1160,10 +1207,11 @@
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="T2 R2 V2 X2 Z2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="U2 S2 W2 Y2 AA2">
       <formula1>"CORRECT,INCORRECT"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>